<commit_message>
add benchmarks for cpu/gpu policy gradient
</commit_message>
<xml_diff>
--- a/marl_4/visualization/marl_benchmark.xlsx
+++ b/marl_4/visualization/marl_benchmark.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\results\marl\visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacky\Desktop\results\marl_4\visualization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{072B4846-10B4-40EA-BC69-7A66BFD7C28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00908812-7C9D-45E8-9627-24A74833823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,31 +36,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">Ray: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">LF:  </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>AWS (100000 episodes, 32 cores, 4 agents)</t>
   </si>
   <si>
-    <t>TrafficJunction 4 Agents</t>
+    <t>Episode:</t>
+  </si>
+  <si>
+    <t>Ray</t>
+  </si>
+  <si>
+    <t>LF</t>
+  </si>
+  <si>
+    <t>Env: TrafficJunction 4 Agents</t>
+  </si>
+  <si>
+    <t>Env: TrafficJunction 10 Agents</t>
+  </si>
+  <si>
+    <t>AWS (10000 episodes, 32 cores, 10 agents)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Ubuntu Mono"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <name val="Ubuntu Mono"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,8 +101,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -365,45 +392,319 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>167.93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B3" s="3">
+        <v>17.79</v>
+      </c>
+      <c r="C3" s="2">
+        <v>7.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <f>A3+10000</f>
+        <v>20000</v>
+      </c>
+      <c r="B4" s="3">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="C4" s="2">
+        <v>14.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <f t="shared" ref="A5:A12" si="0">A4+10000</f>
+        <v>30000</v>
+      </c>
+      <c r="B5" s="3">
+        <v>51.11</v>
+      </c>
+      <c r="C5" s="2">
+        <v>22.32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="B6" s="3">
+        <v>67.97</v>
+      </c>
+      <c r="C6" s="2">
+        <v>29.48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f t="shared" si="0"/>
+        <v>50000</v>
+      </c>
+      <c r="B7" s="3">
+        <v>84.68</v>
+      </c>
+      <c r="C7" s="2">
+        <v>36.54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>101.88</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <f t="shared" si="0"/>
+        <v>70000</v>
+      </c>
+      <c r="B9" s="3">
+        <v>118.74</v>
+      </c>
+      <c r="C9" s="2">
+        <v>50.65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="B10" s="3">
+        <v>135.63999999999999</v>
+      </c>
+      <c r="C10" s="2">
+        <v>57.64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <f t="shared" si="0"/>
+        <v>90000</v>
+      </c>
+      <c r="B11" s="3">
+        <v>152.96</v>
+      </c>
+      <c r="C11" s="2">
+        <v>64.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <f t="shared" si="0"/>
+        <v>100000</v>
+      </c>
+      <c r="B12" s="3">
+        <v>169.52</v>
+      </c>
+      <c r="C12" s="2">
+        <v>71.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>135.63999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>74.459999999999994</v>
-      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>10000</v>
+      </c>
+      <c r="B18" s="3">
+        <v>92.37</v>
+      </c>
+      <c r="C18" s="2">
+        <v>17.87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <f>A18+10000</f>
+        <v>20000</v>
+      </c>
+      <c r="B19" s="3">
+        <v>184.11</v>
+      </c>
+      <c r="C19" s="2">
+        <v>35.799999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <f t="shared" ref="A20:A27" si="1">A19+10000</f>
+        <v>30000</v>
+      </c>
+      <c r="B20" s="3">
+        <v>276.01</v>
+      </c>
+      <c r="C20" s="2">
+        <v>53.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <f t="shared" si="1"/>
+        <v>40000</v>
+      </c>
+      <c r="B21" s="3">
+        <v>367.71</v>
+      </c>
+      <c r="C21" s="2">
+        <v>71.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <f t="shared" si="1"/>
+        <v>50000</v>
+      </c>
+      <c r="B22" s="3">
+        <v>459.01</v>
+      </c>
+      <c r="C22" s="2">
+        <v>89.54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <f t="shared" si="1"/>
+        <v>60000</v>
+      </c>
+      <c r="B23" s="3">
+        <v>550.76</v>
+      </c>
+      <c r="C23" s="2">
+        <v>107.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <f t="shared" si="1"/>
+        <v>70000</v>
+      </c>
+      <c r="B24" s="3">
+        <v>642.29999999999995</v>
+      </c>
+      <c r="C24" s="2">
+        <v>125.41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <f t="shared" si="1"/>
+        <v>80000</v>
+      </c>
+      <c r="B25" s="3">
+        <v>733.73</v>
+      </c>
+      <c r="C25" s="2">
+        <v>143.29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <f t="shared" si="1"/>
+        <v>90000</v>
+      </c>
+      <c r="B26" s="3">
+        <v>825.22</v>
+      </c>
+      <c r="C26" s="2">
+        <v>161.19999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <f t="shared" si="1"/>
+        <v>100000</v>
+      </c>
+      <c r="B27" s="3">
+        <v>917.03</v>
+      </c>
+      <c r="C27" s="2">
+        <v>179.11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>